<commit_message>
Changes to DMD case
</commit_message>
<xml_diff>
--- a/SX DMD case/Clinical Exam/Clinical_Exam_DMDcase.xlsx
+++ b/SX DMD case/Clinical Exam/Clinical_Exam_DMDcase.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0125409\Documents\PhD\7. Congress\SMALL2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GBW_MyPrograms\PredSim-workshop-smalll-2025\SX DMD case\Clinical Exam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBD94CB-FF36-4869-922B-4708CE4F340C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6FD647-AF0C-4DC8-AD0A-320E18C81717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{26813F52-AEA5-49D5-8F25-543231CE14D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{26813F52-AEA5-49D5-8F25-543231CE14D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
-  <si>
-    <t>Hip_add_r_ROM</t>
-  </si>
-  <si>
-    <t>Hip_add_l_ROM</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Hip_ext_r_ROM</t>
   </si>
@@ -50,12 +44,6 @@
     <t>Hip_ext_l_ROM</t>
   </si>
   <si>
-    <t>Knee_ext_r_ROM</t>
-  </si>
-  <si>
-    <t>Knee_ext_l_ROM</t>
-  </si>
-  <si>
     <t>Ham_r_ROM</t>
   </si>
   <si>
@@ -68,18 +56,6 @@
     <t>Ham_l_stiff</t>
   </si>
   <si>
-    <t>RF_r_length</t>
-  </si>
-  <si>
-    <t>RF_l_length</t>
-  </si>
-  <si>
-    <t>RF_r_stiff</t>
-  </si>
-  <si>
-    <t>RF_l_stiff</t>
-  </si>
-  <si>
     <t>Gastroc_r_ROM</t>
   </si>
   <si>
@@ -104,22 +80,10 @@
     <t>Soleus_l_stiff</t>
   </si>
   <si>
-    <t>Hip_add_r_stiff</t>
-  </si>
-  <si>
-    <t>Hip_add_l_stiff</t>
-  </si>
-  <si>
     <t>Hip_ext_r_stiff</t>
   </si>
   <si>
     <t>Hip_ext_l_stiff</t>
-  </si>
-  <si>
-    <t>Knee_ext_r_stiff</t>
-  </si>
-  <si>
-    <t>Knee_ext_l_stiff</t>
   </si>
 </sst>
 </file>
@@ -513,22 +477,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E85F571-1DBF-404A-A902-0FC9F60AAE67}">
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="AA11" sqref="AA11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="8" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="1" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="4" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -536,10 +497,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -548,78 +509,42 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>10</v>
-      </c>
       <c r="B2" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
@@ -627,76 +552,40 @@
       <c r="D2" s="2">
         <v>2</v>
       </c>
-      <c r="E2" s="2">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2">
-        <v>5</v>
-      </c>
-      <c r="G2" s="2">
+      <c r="E2" s="3">
+        <v>-30</v>
+      </c>
+      <c r="F2" s="3">
+        <v>-30</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3">
+        <v>-20</v>
+      </c>
+      <c r="J2" s="3">
+        <v>-20</v>
+      </c>
+      <c r="K2" s="3">
+        <v>3</v>
+      </c>
+      <c r="L2" s="3">
+        <v>3</v>
+      </c>
+      <c r="M2" s="3">
+        <v>-10</v>
+      </c>
+      <c r="N2" s="3">
+        <v>-10</v>
+      </c>
+      <c r="O2" s="2">
         <v>2</v>
       </c>
-      <c r="H2" s="2">
-        <v>2</v>
-      </c>
-      <c r="I2" s="2">
-        <v>5</v>
-      </c>
-      <c r="J2" s="2">
-        <v>5</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2">
-        <v>0</v>
-      </c>
-      <c r="M2" s="3">
-        <v>-30</v>
-      </c>
-      <c r="N2" s="3">
-        <v>-30</v>
-      </c>
-      <c r="O2" s="3">
-        <v>1</v>
-      </c>
-      <c r="P2" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>2</v>
-      </c>
-      <c r="R2" s="3">
-        <v>2</v>
-      </c>
-      <c r="S2" s="3">
-        <v>1</v>
-      </c>
-      <c r="T2" s="3">
-        <v>1</v>
-      </c>
-      <c r="U2" s="3">
-        <v>-20</v>
-      </c>
-      <c r="V2" s="3">
-        <v>-20</v>
-      </c>
-      <c r="W2" s="3">
-        <v>3</v>
-      </c>
-      <c r="X2" s="3">
-        <v>3</v>
-      </c>
-      <c r="Y2" s="3">
-        <v>-10</v>
-      </c>
-      <c r="Z2" s="3">
-        <v>-10</v>
-      </c>
-      <c r="AA2" s="2">
-        <v>2</v>
-      </c>
-      <c r="AB2" s="2">
+      <c r="P2" s="2">
         <v>2</v>
       </c>
     </row>

</xml_diff>